<commit_message>
Move subjective metrics to repo
</commit_message>
<xml_diff>
--- a/data/jod.xlsx
+++ b/data/jod.xlsx
@@ -446,37 +446,37 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>default</t>
+          <t>Default</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>mcmc</t>
+          <t>MCMC</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>mini_splatting</t>
+          <t>Mini-Splatting</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>eagles</t>
+          <t>EAGLES</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mip_splatting</t>
+          <t>Mip-Splatting</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>gaussian_pro</t>
+          <t>Gaussian-Pro</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>geo_gaussian</t>
+          <t>Geo-Gaussian</t>
         </is>
       </c>
     </row>
@@ -495,25 +495,25 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.731665568053696</v>
+        <v>1.224957701347362</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.2440444652521937</v>
+        <v>0.04344177860779775</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.6499223502917386</v>
+        <v>0.009124921513326629</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.5674045996166825</v>
+        <v>-0.9357747657846388</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7550305019657175</v>
+        <v>0.5037227105672092</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.3151215177484488</v>
+        <v>-0.176024416869176</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.7102091075395607</v>
+        <v>-0.6694473619648188</v>
       </c>
     </row>
     <row r="3">
@@ -531,25 +531,25 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-0.04652800630801784</v>
+        <v>0.08460405217332961</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9913564666610233</v>
+        <v>1.091316995387062</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5506813050553151</v>
+        <v>0.588851806290297</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.9565631193926549</v>
+        <v>-1.130979522342304</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7978713290915102</v>
+        <v>0.8466206464111672</v>
       </c>
       <c r="I3" t="n">
-        <v>0.08482484823648093</v>
+        <v>0.1478801253159097</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.421646168173357</v>
+        <v>-1.628307072458627</v>
       </c>
     </row>
     <row r="4">
@@ -567,25 +567,25 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.446036318910741</v>
+        <v>1.508158915403333</v>
       </c>
       <c r="E4" t="n">
-        <v>3.249721891317809</v>
+        <v>3.304051897373304</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.4595598795571639</v>
+        <v>-0.1250320509239081</v>
       </c>
       <c r="G4" t="n">
-        <v>0.09001042499614288</v>
+        <v>-0.2005346945619966</v>
       </c>
       <c r="H4" t="n">
-        <v>-7.040936603895439</v>
+        <v>-7.268493809976309</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2885462391115455</v>
+        <v>0.30435326465208</v>
       </c>
       <c r="J4" t="n">
-        <v>2.426174300620605</v>
+        <v>2.477472606445807</v>
       </c>
     </row>
     <row r="5">
@@ -603,25 +603,25 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-1.671923938125451</v>
+        <v>-2.426513498360832</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.600017777742874</v>
+        <v>-4.119895391172083</v>
       </c>
       <c r="F5" t="n">
-        <v>-10.21815914056578</v>
+        <v>-5.308643137371774</v>
       </c>
       <c r="G5" t="n">
-        <v>6.578660835730119</v>
+        <v>5.98508056837265</v>
       </c>
       <c r="H5" t="n">
-        <v>5.008381805222275</v>
+        <v>4.414793288220697</v>
       </c>
       <c r="I5" t="n">
-        <v>5.563018556802687</v>
+        <v>4.969436954066382</v>
       </c>
       <c r="J5" t="n">
-        <v>-2.65998402534929</v>
+        <v>-3.514271373098783</v>
       </c>
     </row>
     <row r="6">
@@ -639,25 +639,25 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-4.626759028936688</v>
+        <v>-5.231147646353744</v>
       </c>
       <c r="E6" t="n">
-        <v>9.348230128884193</v>
+        <v>10.14639296707296</v>
       </c>
       <c r="F6" t="n">
-        <v>10.59360558522593</v>
+        <v>11.99327157191658</v>
       </c>
       <c r="G6" t="n">
-        <v>-6.123538259248106</v>
+        <v>-6.913766524134874</v>
       </c>
       <c r="H6" t="n">
-        <v>2.689323559377583</v>
+        <v>2.800127194568744</v>
       </c>
       <c r="I6" t="n">
-        <v>-5.540717006844678</v>
+        <v>-6.085657373506661</v>
       </c>
       <c r="J6" t="n">
-        <v>-6.340170752342152</v>
+        <v>-6.709242611018718</v>
       </c>
     </row>
     <row r="7">
@@ -675,25 +675,25 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-1.888787866743014</v>
+        <v>-1.899611007026507</v>
       </c>
       <c r="E7" t="n">
-        <v>6.307277874179712</v>
+        <v>6.334340827854865</v>
       </c>
       <c r="F7" t="n">
-        <v>-2.340323277528341</v>
+        <v>-2.351148186562976</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.57669387242201</v>
+        <v>-1.587518152405999</v>
       </c>
       <c r="H7" t="n">
-        <v>5.353412722404483</v>
+        <v>5.380464729201268</v>
       </c>
       <c r="I7" t="n">
-        <v>-3.18339411003622</v>
+        <v>-3.194217674659312</v>
       </c>
       <c r="J7" t="n">
-        <v>-2.67152499803721</v>
+        <v>-2.682347832757456</v>
       </c>
     </row>
     <row r="8">
@@ -747,25 +747,25 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-0.3337118933837557</v>
+        <v>-0.1129042907591787</v>
       </c>
       <c r="E9" t="n">
-        <v>1.024160795112071</v>
+        <v>1.346946205933439</v>
       </c>
       <c r="F9" t="n">
-        <v>2.55825398489183</v>
+        <v>3.049268828132393</v>
       </c>
       <c r="G9" t="n">
-        <v>1.194360518421995</v>
+        <v>1.452908118253542</v>
       </c>
       <c r="H9" t="n">
-        <v>1.931808973583581</v>
+        <v>2.254115055176811</v>
       </c>
       <c r="I9" t="n">
-        <v>0.7824069931276066</v>
+        <v>1.004839533414738</v>
       </c>
       <c r="J9" t="n">
-        <v>-7.157311001687167</v>
+        <v>-8.995284166447723</v>
       </c>
     </row>
     <row r="10">
@@ -783,25 +783,25 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-0.5493595016214221</v>
+        <v>-0.6004657316353234</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.9166371412467167</v>
+        <v>-0.5840946745515707</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.4302802573320551</v>
+        <v>-0.3202807595768558</v>
       </c>
       <c r="G10" t="n">
-        <v>2.066036716132562</v>
+        <v>1.905476895875601</v>
       </c>
       <c r="H10" t="n">
-        <v>0.8724798800754472</v>
+        <v>0.5281051897351202</v>
       </c>
       <c r="I10" t="n">
-        <v>1.056086684921205</v>
+        <v>1.03334950061445</v>
       </c>
       <c r="J10" t="n">
-        <v>-2.098330227308984</v>
+        <v>-1.962093278318804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>